<commit_message>
Updates reference database and reruns assigntaxonomy and phyloseq for plate 1
</commit_message>
<xml_diff>
--- a/SRKW-diet-16SP1.xlsx
+++ b/SRKW-diet-16SP1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/SRKW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="11_1480BCC88F79A8D366075C52F37BD2725ACE99EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB7B27CE-2D24-49F7-AEF2-B93937992635}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="11_1480BCC88F79A8D366075C52F37BD2725ACE99EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E95E470-6275-4B28-B985-A74034B3880A}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3541" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3546" uniqueCount="521">
   <si>
     <t>rownames</t>
   </si>
@@ -1569,13 +1569,28 @@
   </si>
   <si>
     <t>100% Oncorhynchus tshawytscha, Oncorhynchus nerka</t>
+  </si>
+  <si>
+    <t>Notes on refdb</t>
+  </si>
+  <si>
+    <t>added as O.spp.</t>
+  </si>
+  <si>
+    <t>HAVE NOT ADDED  buit all are in pleuronectiformes and pleuronectidae</t>
+  </si>
+  <si>
+    <t>added as O. spp.</t>
+  </si>
+  <si>
+    <t>sdfgsdfsdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1593,18 +1608,35 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF212121"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1616,18 +1648,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1641,6 +1678,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1932,8 +1973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H442"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A415" workbookViewId="0">
+      <selection activeCell="A442" sqref="A442"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12891,7 +12932,7 @@
     </row>
     <row r="442" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>497</v>
+        <v>520</v>
       </c>
       <c r="B442" t="s">
         <v>9</v>
@@ -12919,10 +12960,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8817D8-A495-4FD3-ABA5-1238E17F2939}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12935,9 +12976,10 @@
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" customWidth="1"/>
     <col min="9" max="9" width="44.42578125" customWidth="1"/>
+    <col min="10" max="10" width="52.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12968,16 +13010,19 @@
       <c r="J1" s="1" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="K1" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -12985,7 +13030,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -13002,119 +13047,122 @@
         <v>501</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="3" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="K7" s="3" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>281</v>
       </c>
@@ -13134,52 +13182,52 @@
         <v>508</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="2" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>329</v>
       </c>
@@ -13196,361 +13244,370 @@
         <v>510</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="K20" s="3" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="B22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="K22" s="3" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="2" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="B24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="B24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="2" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="B25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="2" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="B26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="2" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="2" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="B28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="B28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="2" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="B30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="B30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="2" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="B33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="B33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="2" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="I35" s="4" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="K35" s="3" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="2" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="B37" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" t="s">
-        <v>14</v>
-      </c>
-      <c r="I37" t="s">
+      <c r="B37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" s="2" t="s">
         <v>504</v>
       </c>
     </row>

</xml_diff>